<commit_message>
added name for nomura broker
</commit_message>
<xml_diff>
--- a/reference/SSI2019.xlsx
+++ b/reference/SSI2019.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhangst\git\boci_trustee\reference\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steven.zhang\AppData\Local\Programs\Git\git\boci_trustee\reference\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2788CC6-FA20-4A19-A66C-83BB799E6D97}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6318310E-75D5-4DE8-9908-B27DF4EB096E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{604E8566-0329-48B3-9E88-978878A4F528}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{604E8566-0329-48B3-9E88-978878A4F528}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="142">
   <si>
     <t>Broker Id</t>
   </si>
@@ -454,6 +454,12 @@
   </si>
   <si>
     <t>18800</t>
+  </si>
+  <si>
+    <t>NOMX-FI</t>
+  </si>
+  <si>
+    <t>NOMX-FI is INST-FI</t>
   </si>
 </sst>
 </file>
@@ -814,22 +820,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B3908C6-0BF6-4931-B932-632D6D3B8514}">
-  <dimension ref="A1:E36"/>
+  <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -846,7 +852,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -863,7 +869,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -880,7 +886,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>26</v>
       </c>
@@ -897,7 +903,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -914,7 +920,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>56</v>
       </c>
@@ -931,7 +937,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>31</v>
       </c>
@@ -948,7 +954,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>31</v>
       </c>
@@ -965,7 +971,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>60</v>
       </c>
@@ -982,7 +988,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>48</v>
       </c>
@@ -999,7 +1005,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>36</v>
       </c>
@@ -1016,7 +1022,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>44</v>
       </c>
@@ -1033,7 +1039,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>40</v>
       </c>
@@ -1050,7 +1056,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>52</v>
       </c>
@@ -1067,7 +1073,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>64</v>
       </c>
@@ -1084,7 +1090,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>72</v>
       </c>
@@ -1101,7 +1107,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>68</v>
       </c>
@@ -1118,7 +1124,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>132</v>
       </c>
@@ -1135,7 +1141,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>76</v>
       </c>
@@ -1152,7 +1158,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>80</v>
       </c>
@@ -1169,7 +1175,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>84</v>
       </c>
@@ -1186,7 +1192,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>112</v>
       </c>
@@ -1203,41 +1209,44 @@
         <v>115</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>140</v>
+      </c>
+      <c r="B23" t="s">
+        <v>113</v>
+      </c>
+      <c r="C23" t="s">
+        <v>114</v>
+      </c>
+      <c r="D23" t="s">
+        <v>8</v>
+      </c>
+      <c r="E23" t="s">
+        <v>115</v>
+      </c>
+      <c r="G23" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>88</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B24" t="s">
         <v>89</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C24" t="s">
         <v>90</v>
       </c>
-      <c r="D23" t="s">
-        <v>8</v>
-      </c>
-      <c r="E23" t="s">
+      <c r="D24" t="s">
+        <v>8</v>
+      </c>
+      <c r="E24" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>92</v>
-      </c>
-      <c r="B24" t="s">
-        <v>93</v>
-      </c>
-      <c r="C24" t="s">
-        <v>94</v>
-      </c>
-      <c r="D24" t="s">
-        <v>8</v>
-      </c>
-      <c r="E24" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>92</v>
       </c>
@@ -1245,21 +1254,21 @@
         <v>93</v>
       </c>
       <c r="C25" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D25" t="s">
         <v>8</v>
       </c>
       <c r="E25" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>92</v>
       </c>
       <c r="B26" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C26" t="s">
         <v>96</v>
@@ -1268,182 +1277,199 @@
         <v>8</v>
       </c>
       <c r="E26" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>92</v>
+      </c>
+      <c r="B27" t="s">
+        <v>98</v>
+      </c>
+      <c r="C27" t="s">
+        <v>96</v>
+      </c>
+      <c r="D27" t="s">
+        <v>8</v>
+      </c>
+      <c r="E27" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>100</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B28" t="s">
         <v>101</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C28" t="s">
         <v>102</v>
       </c>
-      <c r="D27" t="s">
-        <v>8</v>
-      </c>
-      <c r="E27" t="s">
+      <c r="D28" t="s">
+        <v>8</v>
+      </c>
+      <c r="E28" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>5</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B29" t="s">
         <v>6</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C29" t="s">
         <v>7</v>
       </c>
-      <c r="D28" t="s">
-        <v>8</v>
-      </c>
-      <c r="E28" t="s">
+      <c r="D29" t="s">
+        <v>8</v>
+      </c>
+      <c r="E29" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>108</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B30" t="s">
         <v>109</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C30" t="s">
         <v>110</v>
       </c>
-      <c r="D29" t="s">
-        <v>8</v>
-      </c>
-      <c r="E29" t="s">
+      <c r="D30" t="s">
+        <v>8</v>
+      </c>
+      <c r="E30" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>104</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B31" t="s">
         <v>105</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C31" t="s">
         <v>106</v>
       </c>
-      <c r="D30" t="s">
-        <v>8</v>
-      </c>
-      <c r="E30" t="s">
+      <c r="D31" t="s">
+        <v>8</v>
+      </c>
+      <c r="E31" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>116</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B32" t="s">
         <v>117</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C32" t="s">
         <v>118</v>
       </c>
-      <c r="D31" t="s">
-        <v>8</v>
-      </c>
-      <c r="E31" t="s">
+      <c r="D32" t="s">
+        <v>8</v>
+      </c>
+      <c r="E32" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>10</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B33" t="s">
         <v>11</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C33" t="s">
         <v>12</v>
       </c>
-      <c r="D32" t="s">
-        <v>8</v>
-      </c>
-      <c r="E32" t="s">
+      <c r="D33" t="s">
+        <v>8</v>
+      </c>
+      <c r="E33" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>124</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B34" t="s">
         <v>125</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C34" t="s">
         <v>126</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D34" t="s">
         <v>29</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E34" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>120</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B35" t="s">
         <v>121</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C35" t="s">
         <v>122</v>
       </c>
-      <c r="D34" t="s">
-        <v>8</v>
-      </c>
-      <c r="E34" t="s">
+      <c r="D35" t="s">
+        <v>8</v>
+      </c>
+      <c r="E35" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>128</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B36" t="s">
         <v>129</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C36" t="s">
         <v>130</v>
       </c>
-      <c r="D35" t="s">
-        <v>8</v>
-      </c>
-      <c r="E35" t="s">
+      <c r="D36" t="s">
+        <v>8</v>
+      </c>
+      <c r="E36" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>136</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B37" t="s">
         <v>137</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C37" t="s">
         <v>138</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D37" t="s">
         <v>29</v>
       </c>
-      <c r="E36" t="s">
+      <c r="E37" t="s">
         <v>139</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E36">
-    <sortCondition ref="A1:A36"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E37">
+    <sortCondition ref="A1:A37"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
updated SSI reference file for nomura
</commit_message>
<xml_diff>
--- a/reference/SSI2019.xlsx
+++ b/reference/SSI2019.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steven.zhang\AppData\Local\Programs\Git\git\boci_trustee\reference\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6318310E-75D5-4DE8-9908-B27DF4EB096E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D314D2F6-C352-4E30-A757-3984A699335A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{604E8566-0329-48B3-9E88-978878A4F528}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="17445" windowHeight="14565" xr2:uid="{604E8566-0329-48B3-9E88-978878A4F528}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="141">
   <si>
     <t>Broker Id</t>
   </si>
@@ -457,9 +457,6 @@
   </si>
   <si>
     <t>NOMX-FI</t>
-  </si>
-  <si>
-    <t>NOMX-FI is INST-FI</t>
   </si>
 </sst>
 </file>
@@ -820,10 +817,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B3908C6-0BF6-4931-B932-632D6D3B8514}">
-  <dimension ref="A1:G37"/>
+  <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1107,7 +1104,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>68</v>
       </c>
@@ -1124,7 +1121,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>132</v>
       </c>
@@ -1141,7 +1138,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>76</v>
       </c>
@@ -1158,7 +1155,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>80</v>
       </c>
@@ -1175,7 +1172,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>84</v>
       </c>
@@ -1192,7 +1189,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>112</v>
       </c>
@@ -1209,7 +1206,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>140</v>
       </c>
@@ -1225,11 +1222,8 @@
       <c r="E23" t="s">
         <v>115</v>
       </c>
-      <c r="G23" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>88</v>
       </c>
@@ -1246,7 +1240,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>92</v>
       </c>
@@ -1263,7 +1257,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>92</v>
       </c>
@@ -1280,7 +1274,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>92</v>
       </c>
@@ -1297,7 +1291,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>100</v>
       </c>
@@ -1314,7 +1308,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>5</v>
       </c>
@@ -1331,7 +1325,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>108</v>
       </c>
@@ -1348,7 +1342,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>104</v>
       </c>
@@ -1365,7 +1359,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>116</v>
       </c>

</xml_diff>

<commit_message>
updated credit suisse SSI
</commit_message>
<xml_diff>
--- a/reference/SSI2019.xlsx
+++ b/reference/SSI2019.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steven.zhang\AppData\Local\Programs\Git\git\boci_trustee\reference\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B3486FB-EFA6-4FE8-9769-A0BF7202C041}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BEDBCA8-5DD0-40A6-964F-C1BDC329512B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{604E8566-0329-48B3-9E88-978878A4F528}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="147">
   <si>
     <t>Broker Id</t>
   </si>
@@ -175,9 +175,6 @@
   </si>
   <si>
     <t>CSFBGB2LXXX</t>
-  </si>
-  <si>
-    <t>93827</t>
   </si>
   <si>
     <t>CICC-FI</t>
@@ -521,9 +518,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -840,8 +838,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B3908C6-0BF6-4931-B932-632D6D3B8514}">
   <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="J31" sqref="J31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -940,19 +938,19 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B6" t="s">
         <v>56</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>57</v>
-      </c>
-      <c r="C6" t="s">
-        <v>58</v>
       </c>
       <c r="D6" t="s">
         <v>29</v>
       </c>
       <c r="E6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -991,36 +989,36 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B9" t="s">
         <v>60</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>61</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" t="s">
         <v>62</v>
-      </c>
-      <c r="D9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" t="s">
         <v>48</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>49</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" t="s">
         <v>50</v>
-      </c>
-      <c r="D10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1053,8 +1051,8 @@
       <c r="D12" t="s">
         <v>8</v>
       </c>
-      <c r="E12" t="s">
-        <v>47</v>
+      <c r="E12" s="2">
+        <v>94673</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1076,257 +1074,257 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>51</v>
+      </c>
+      <c r="B14" t="s">
         <v>52</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>53</v>
-      </c>
-      <c r="C14" t="s">
-        <v>54</v>
       </c>
       <c r="D14" t="s">
         <v>29</v>
       </c>
       <c r="E14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15" t="s">
         <v>64</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>65</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" t="s">
         <v>66</v>
-      </c>
-      <c r="D15" t="s">
-        <v>8</v>
-      </c>
-      <c r="E15" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>71</v>
+      </c>
+      <c r="B16" t="s">
         <v>72</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>73</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" t="s">
         <v>74</v>
-      </c>
-      <c r="D16" t="s">
-        <v>8</v>
-      </c>
-      <c r="E16" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>67</v>
+      </c>
+      <c r="B17" t="s">
         <v>68</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>69</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" t="s">
         <v>70</v>
-      </c>
-      <c r="D17" t="s">
-        <v>8</v>
-      </c>
-      <c r="E17" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>131</v>
+      </c>
+      <c r="B18" t="s">
         <v>132</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>133</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" t="s">
         <v>134</v>
-      </c>
-      <c r="D18" t="s">
-        <v>8</v>
-      </c>
-      <c r="E18" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>75</v>
+      </c>
+      <c r="B19" t="s">
         <v>76</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>77</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" t="s">
         <v>78</v>
-      </c>
-      <c r="D19" t="s">
-        <v>8</v>
-      </c>
-      <c r="E19" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>79</v>
+      </c>
+      <c r="B20" t="s">
         <v>80</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>81</v>
-      </c>
-      <c r="C20" t="s">
-        <v>82</v>
       </c>
       <c r="D20" t="s">
         <v>29</v>
       </c>
       <c r="E20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>83</v>
+      </c>
+      <c r="B21" t="s">
         <v>84</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>85</v>
-      </c>
-      <c r="C21" t="s">
-        <v>86</v>
       </c>
       <c r="D21" t="s">
         <v>29</v>
       </c>
       <c r="E21" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>111</v>
+      </c>
+      <c r="B22" t="s">
         <v>112</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>113</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
+        <v>8</v>
+      </c>
+      <c r="E22" t="s">
         <v>114</v>
-      </c>
-      <c r="D22" t="s">
-        <v>8</v>
-      </c>
-      <c r="E22" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B23" t="s">
+        <v>112</v>
+      </c>
+      <c r="C23" t="s">
         <v>113</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
+        <v>8</v>
+      </c>
+      <c r="E23" t="s">
         <v>114</v>
-      </c>
-      <c r="D23" t="s">
-        <v>8</v>
-      </c>
-      <c r="E23" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>87</v>
+      </c>
+      <c r="B24" t="s">
         <v>88</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>89</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
+        <v>8</v>
+      </c>
+      <c r="E24" t="s">
         <v>90</v>
-      </c>
-      <c r="D24" t="s">
-        <v>8</v>
-      </c>
-      <c r="E24" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>91</v>
+      </c>
+      <c r="B25" t="s">
         <v>92</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
         <v>93</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
+        <v>8</v>
+      </c>
+      <c r="E25" t="s">
         <v>94</v>
-      </c>
-      <c r="D25" t="s">
-        <v>8</v>
-      </c>
-      <c r="E25" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>91</v>
+      </c>
+      <c r="B26" t="s">
         <v>92</v>
       </c>
-      <c r="B26" t="s">
-        <v>93</v>
-      </c>
       <c r="C26" t="s">
+        <v>95</v>
+      </c>
+      <c r="D26" t="s">
+        <v>8</v>
+      </c>
+      <c r="E26" t="s">
         <v>96</v>
-      </c>
-      <c r="D26" t="s">
-        <v>8</v>
-      </c>
-      <c r="E26" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B27" t="s">
+        <v>97</v>
+      </c>
+      <c r="C27" t="s">
+        <v>95</v>
+      </c>
+      <c r="D27" t="s">
+        <v>8</v>
+      </c>
+      <c r="E27" t="s">
         <v>98</v>
-      </c>
-      <c r="C27" t="s">
-        <v>96</v>
-      </c>
-      <c r="D27" t="s">
-        <v>8</v>
-      </c>
-      <c r="E27" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>99</v>
+      </c>
+      <c r="B28" t="s">
         <v>100</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" t="s">
         <v>101</v>
       </c>
-      <c r="C28" t="s">
+      <c r="D28" t="s">
+        <v>8</v>
+      </c>
+      <c r="E28" t="s">
         <v>102</v>
-      </c>
-      <c r="D28" t="s">
-        <v>8</v>
-      </c>
-      <c r="E28" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -1348,53 +1346,53 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>107</v>
+      </c>
+      <c r="B30" t="s">
         <v>108</v>
       </c>
-      <c r="B30" t="s">
+      <c r="C30" t="s">
         <v>109</v>
       </c>
-      <c r="C30" t="s">
+      <c r="D30" t="s">
+        <v>8</v>
+      </c>
+      <c r="E30" t="s">
         <v>110</v>
-      </c>
-      <c r="D30" t="s">
-        <v>8</v>
-      </c>
-      <c r="E30" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>103</v>
+      </c>
+      <c r="B31" t="s">
         <v>104</v>
       </c>
-      <c r="B31" t="s">
+      <c r="C31" t="s">
         <v>105</v>
       </c>
-      <c r="C31" t="s">
+      <c r="D31" t="s">
+        <v>8</v>
+      </c>
+      <c r="E31" t="s">
         <v>106</v>
-      </c>
-      <c r="D31" t="s">
-        <v>8</v>
-      </c>
-      <c r="E31" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>115</v>
+      </c>
+      <c r="B32" t="s">
         <v>116</v>
       </c>
-      <c r="B32" t="s">
+      <c r="C32" t="s">
         <v>117</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D32" t="s">
+        <v>8</v>
+      </c>
+      <c r="E32" t="s">
         <v>118</v>
-      </c>
-      <c r="D32" t="s">
-        <v>8</v>
-      </c>
-      <c r="E32" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -1416,101 +1414,101 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>123</v>
+      </c>
+      <c r="B34" t="s">
         <v>124</v>
       </c>
-      <c r="B34" t="s">
+      <c r="C34" t="s">
         <v>125</v>
-      </c>
-      <c r="C34" t="s">
-        <v>126</v>
       </c>
       <c r="D34" t="s">
         <v>29</v>
       </c>
       <c r="E34" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>119</v>
+      </c>
+      <c r="B35" t="s">
         <v>120</v>
       </c>
-      <c r="B35" t="s">
+      <c r="C35" t="s">
         <v>121</v>
       </c>
-      <c r="C35" t="s">
+      <c r="D35" t="s">
+        <v>8</v>
+      </c>
+      <c r="E35" t="s">
         <v>122</v>
-      </c>
-      <c r="D35" t="s">
-        <v>8</v>
-      </c>
-      <c r="E35" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>127</v>
+      </c>
+      <c r="B36" t="s">
         <v>128</v>
       </c>
-      <c r="B36" t="s">
+      <c r="C36" t="s">
         <v>129</v>
       </c>
-      <c r="C36" t="s">
+      <c r="D36" t="s">
+        <v>8</v>
+      </c>
+      <c r="E36" t="s">
         <v>130</v>
-      </c>
-      <c r="D36" t="s">
-        <v>8</v>
-      </c>
-      <c r="E36" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>135</v>
+      </c>
+      <c r="B37" t="s">
         <v>136</v>
       </c>
-      <c r="B37" t="s">
+      <c r="C37" t="s">
         <v>137</v>
-      </c>
-      <c r="C37" t="s">
-        <v>138</v>
       </c>
       <c r="D37" t="s">
         <v>29</v>
       </c>
       <c r="E37" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>140</v>
+      </c>
+      <c r="B38" t="s">
         <v>141</v>
       </c>
-      <c r="B38" t="s">
+      <c r="C38" t="s">
         <v>142</v>
-      </c>
-      <c r="C38" t="s">
-        <v>143</v>
       </c>
       <c r="D38" t="s">
         <v>29</v>
       </c>
       <c r="E38" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>144</v>
+      </c>
+      <c r="B39" t="s">
         <v>145</v>
-      </c>
-      <c r="B39" t="s">
-        <v>146</v>
       </c>
       <c r="D39" t="s">
         <v>29</v>
       </c>
       <c r="E39" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
   </sheetData>

</xml_diff>